<commit_message>
Updates made to save changes completed today
</commit_message>
<xml_diff>
--- a/data/raw/realestate.xlsx
+++ b/data/raw/realestate.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\saidmf\Desktop\TKH\rental-pricing-explore\data\raw\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\deema\Desktop\TKH\Rental-Predictions-Taipei-City\data\raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{178BDDDD-7CA3-4FD9-BC0C-DA67D2CCBA2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39AB719F-6EC7-4794-83EC-E14ADB381582}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="工作表1" sheetId="1" r:id="rId1"/>
@@ -1229,17 +1229,17 @@
   <dimension ref="A1:G415"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A18" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1:H1048576"/>
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.5"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="8.9140625" style="1"/>
+    <col min="1" max="1" width="8.875" style="1"/>
     <col min="2" max="6" width="30.75" style="1" customWidth="1"/>
-    <col min="7" max="7" width="31.08203125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="31.125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="18.5">
+    <row r="1" spans="1:7" ht="18.75">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>

</xml_diff>